<commit_message>
delete initial data for all rows
</commit_message>
<xml_diff>
--- a/RAPPORT-BUDGET-FONCT-2024.xlsx
+++ b/RAPPORT-BUDGET-FONCT-2024.xlsx
@@ -1909,8 +1909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R1348"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="F43" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="I84" sqref="I84"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="G1328" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="I1340" activeCellId="159" sqref="I464:Q464 I472 I480:I481 I490 I496 I500 I506 I513 I524 I527 I535 I544 I550 I559 I573 I577 I586 I592 I598 I602 I610 I620 I626 I634 I642 I647 I655 I667 I675 I673 I679 I683 I688 I698 I695 I706 I763 I771 I784 I785 I789 I793 I799 I800 I803 I809 I817 I822 I827 I835 I838 I843 I849 I856 I858 I866 I868 I875 I882 I888 I890 I893 I898 I904 I908 I913 I917 I923 I927 I933 I937 I943 I947 I952 I955 I959 I966 I974 I981 I982 I984 I987 I990 I998 I1005 I1007 I1008 I1009 I1011 I1013 I1015 I1021 I1023 I1025 I1027 I1029 I1032 I1034 I1036 I1038 I1040 I1042 I1044 I1064 I1070 I1076 I1079 I1082 I1085 I1090 I1095 I1100 I1104 I1107 I1110 I1113 I1116 I1119 I1126 I1128 I1129 I1130 I1131 I1133 I1134 I1136 I1137 I1138 I1139 I1140 I1159 I1167 I1175 I1182 I1185 I1193 I1201 I1209 I1217 I1223 I1227 I1238 I1244 I1250 I1256 I1262 I1268 I1274 I1280 I1286 I1291 I1295 I1305 I1306 I1314 I1322 I1327 I1328 I1334 I1340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="18.5" x14ac:dyDescent="0.65"/>
@@ -2170,25 +2170,15 @@
       <c r="H10" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="37">
-        <v>386300</v>
-      </c>
+      <c r="I10" s="37"/>
       <c r="J10" s="37"/>
-      <c r="K10" s="30">
-        <f>SUM(I10:J10)</f>
-        <v>386300</v>
-      </c>
+      <c r="K10" s="30"/>
       <c r="L10" s="37"/>
       <c r="M10" s="37"/>
       <c r="N10" s="37"/>
       <c r="O10" s="37"/>
-      <c r="P10" s="37">
-        <v>386300</v>
-      </c>
-      <c r="Q10" s="30">
-        <f t="shared" ref="Q10:Q28" si="0">SUM(L10-N10)</f>
-        <v>0</v>
-      </c>
+      <c r="P10" s="37"/>
+      <c r="Q10" s="30"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="31"/>
@@ -2795,25 +2785,15 @@
       <c r="H27" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="I27" s="37">
-        <v>3052900</v>
-      </c>
+      <c r="I27" s="37"/>
       <c r="J27" s="37"/>
-      <c r="K27" s="30">
-        <f t="shared" ref="K27:K28" si="1">SUM(I27:J27)</f>
-        <v>3052900</v>
-      </c>
+      <c r="K27" s="30"/>
       <c r="L27" s="37"/>
       <c r="M27" s="37"/>
       <c r="N27" s="37"/>
       <c r="O27" s="37"/>
-      <c r="P27" s="37">
-        <v>3052900</v>
-      </c>
-      <c r="Q27" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="P27" s="37"/>
+      <c r="Q27" s="30"/>
     </row>
     <row r="28" spans="1:17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="38"/>
@@ -2828,25 +2808,15 @@
       <c r="H28" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="I28" s="37">
-        <v>4566800</v>
-      </c>
+      <c r="I28" s="37"/>
       <c r="J28" s="37"/>
-      <c r="K28" s="30">
-        <f t="shared" si="1"/>
-        <v>4566800</v>
-      </c>
+      <c r="K28" s="30"/>
       <c r="L28" s="37"/>
       <c r="M28" s="37"/>
       <c r="N28" s="37"/>
       <c r="O28" s="37"/>
-      <c r="P28" s="37">
-        <v>4566800</v>
-      </c>
-      <c r="Q28" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="P28" s="37"/>
+      <c r="Q28" s="30"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="31"/>
@@ -3458,35 +3428,35 @@
         <v>5157783.93</v>
       </c>
       <c r="J45" s="5">
-        <f t="shared" ref="J45:Q45" si="2">SUM(J29:J44,J11:J26)</f>
+        <f t="shared" ref="J45:Q45" si="0">SUM(J29:J44,J11:J26)</f>
         <v>125795.20000000001</v>
       </c>
       <c r="K45" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5283579.13</v>
       </c>
       <c r="L45" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5107693.4300000006</v>
       </c>
       <c r="M45" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1650</v>
       </c>
       <c r="N45" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5107693.33</v>
       </c>
       <c r="O45" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1650</v>
       </c>
       <c r="P45" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>174235.6999999999</v>
       </c>
       <c r="Q45" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.10000000006220944</v>
       </c>
     </row>
@@ -3506,35 +3476,35 @@
         <v>5157783.93</v>
       </c>
       <c r="J46" s="3">
-        <f t="shared" ref="J46:Q46" si="3">J45</f>
+        <f t="shared" ref="J46:Q46" si="1">J45</f>
         <v>125795.20000000001</v>
       </c>
       <c r="K46" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>5283579.13</v>
       </c>
       <c r="L46" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>5107693.4300000006</v>
       </c>
       <c r="M46" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1650</v>
       </c>
       <c r="N46" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>5107693.33</v>
       </c>
       <c r="O46" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1650</v>
       </c>
       <c r="P46" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>174235.6999999999</v>
       </c>
       <c r="Q46" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.10000000006220944</v>
       </c>
     </row>
@@ -3597,27 +3567,15 @@
       <c r="H49" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="I49" s="37">
-        <f>367900+5400</f>
-        <v>373300</v>
-      </c>
+      <c r="I49" s="37"/>
       <c r="J49" s="37"/>
-      <c r="K49" s="37">
-        <f t="shared" ref="K49:K70" si="4">SUM(I49:J49)</f>
-        <v>373300</v>
-      </c>
+      <c r="K49" s="37"/>
       <c r="L49" s="37"/>
       <c r="M49" s="37"/>
       <c r="N49" s="37"/>
       <c r="O49" s="37"/>
-      <c r="P49" s="37">
-        <f t="shared" ref="P49" si="5">367900+5400</f>
-        <v>373300</v>
-      </c>
-      <c r="Q49" s="30">
-        <f t="shared" ref="Q49:Q70" si="6">SUM(L49-N49)</f>
-        <v>0</v>
-      </c>
+      <c r="P49" s="37"/>
+      <c r="Q49" s="30"/>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="31"/>
@@ -4080,25 +4038,15 @@
       <c r="H62" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="I62" s="37">
-        <v>2044200</v>
-      </c>
+      <c r="I62" s="37"/>
       <c r="J62" s="37"/>
-      <c r="K62" s="37">
-        <f t="shared" si="4"/>
-        <v>2044200</v>
-      </c>
+      <c r="K62" s="37"/>
       <c r="L62" s="37"/>
       <c r="M62" s="37"/>
       <c r="N62" s="37"/>
       <c r="O62" s="37"/>
-      <c r="P62" s="37">
-        <v>2044200</v>
-      </c>
-      <c r="Q62" s="30">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
+      <c r="P62" s="37"/>
+      <c r="Q62" s="30"/>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="31"/>
@@ -4378,25 +4326,15 @@
       <c r="H70" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="I70" s="37">
-        <v>4053500</v>
-      </c>
+      <c r="I70" s="37"/>
       <c r="J70" s="37"/>
-      <c r="K70" s="37">
-        <f t="shared" si="4"/>
-        <v>4053500</v>
-      </c>
+      <c r="K70" s="37"/>
       <c r="L70" s="37"/>
       <c r="M70" s="37"/>
       <c r="N70" s="37"/>
       <c r="O70" s="37"/>
-      <c r="P70" s="37">
-        <v>4053500</v>
-      </c>
-      <c r="Q70" s="30">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
+      <c r="P70" s="37"/>
+      <c r="Q70" s="30"/>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="38"/>
@@ -4858,35 +4796,35 @@
         <v>5193800</v>
       </c>
       <c r="J83" s="5">
-        <f t="shared" ref="J83:Q83" si="7">SUM(J71:J82,J63:J69,J50:J61)</f>
+        <f t="shared" ref="J83:Q83" si="2">SUM(J71:J82,J63:J69,J50:J61)</f>
         <v>0</v>
       </c>
       <c r="K83" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>5193800</v>
       </c>
       <c r="L83" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>4968083.8600000003</v>
       </c>
       <c r="M83" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N83" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>4968083.8600000003</v>
       </c>
       <c r="O83" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P83" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>225716.1399999999</v>
       </c>
       <c r="Q83" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4906,35 +4844,35 @@
         <v>5193800</v>
       </c>
       <c r="J84" s="3">
-        <f t="shared" ref="J84:Q84" si="8">J83</f>
+        <f t="shared" ref="J84:Q84" si="3">J83</f>
         <v>0</v>
       </c>
       <c r="K84" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>5193800</v>
       </c>
       <c r="L84" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>4968083.8600000003</v>
       </c>
       <c r="M84" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N84" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>4968083.8600000003</v>
       </c>
       <c r="O84" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P84" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>225716.1399999999</v>
       </c>
       <c r="Q84" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -4997,25 +4935,15 @@
       <c r="H87" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="I87" s="37">
-        <v>68000</v>
-      </c>
+      <c r="I87" s="37"/>
       <c r="J87" s="37"/>
-      <c r="K87" s="37">
-        <f t="shared" ref="K87:K229" si="9">SUM(I87:J87)</f>
-        <v>68000</v>
-      </c>
+      <c r="K87" s="37"/>
       <c r="L87" s="37"/>
       <c r="M87" s="37"/>
       <c r="N87" s="37"/>
       <c r="O87" s="37"/>
-      <c r="P87" s="37">
-        <v>68000</v>
-      </c>
-      <c r="Q87" s="30">
-        <f t="shared" ref="Q87:Q229" si="10">SUM(L87-N87)</f>
-        <v>0</v>
-      </c>
+      <c r="P87" s="37"/>
+      <c r="Q87" s="30"/>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A88" s="31"/>
@@ -5163,7 +5091,7 @@
       </c>
       <c r="J92" s="37"/>
       <c r="K92" s="37">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="K87:K229" si="4">SUM(I92:J92)</f>
         <v>62000</v>
       </c>
       <c r="L92" s="37"/>
@@ -5174,7 +5102,7 @@
         <v>62000</v>
       </c>
       <c r="Q92" s="30">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="Q87:Q229" si="5">SUM(L92-N92)</f>
         <v>0</v>
       </c>
     </row>
@@ -5408,25 +5336,15 @@
       <c r="H100" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="I100" s="37">
-        <v>5400</v>
-      </c>
+      <c r="I100" s="37"/>
       <c r="J100" s="37"/>
-      <c r="K100" s="37">
-        <f t="shared" si="9"/>
-        <v>5400</v>
-      </c>
+      <c r="K100" s="37"/>
       <c r="L100" s="37"/>
       <c r="M100" s="37"/>
       <c r="N100" s="37"/>
       <c r="O100" s="37"/>
-      <c r="P100" s="37">
-        <v>5400</v>
-      </c>
-      <c r="Q100" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
+      <c r="P100" s="37"/>
+      <c r="Q100" s="30"/>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A101" s="31"/>
@@ -5645,25 +5563,15 @@
       <c r="H107" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="I107" s="37">
-        <v>37600</v>
-      </c>
+      <c r="I107" s="37"/>
       <c r="J107" s="37"/>
-      <c r="K107" s="37">
-        <f t="shared" si="9"/>
-        <v>37600</v>
-      </c>
+      <c r="K107" s="37"/>
       <c r="L107" s="37"/>
       <c r="M107" s="37"/>
       <c r="N107" s="37"/>
       <c r="O107" s="37"/>
-      <c r="P107" s="37">
-        <v>37600</v>
-      </c>
-      <c r="Q107" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
+      <c r="P107" s="37"/>
+      <c r="Q107" s="30"/>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A108" s="31"/>
@@ -6114,25 +6022,15 @@
       <c r="H120" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="I120" s="37">
-        <v>0</v>
-      </c>
+      <c r="I120" s="37"/>
       <c r="J120" s="37"/>
-      <c r="K120" s="37">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
+      <c r="K120" s="37"/>
       <c r="L120" s="37"/>
       <c r="M120" s="37"/>
       <c r="N120" s="37"/>
       <c r="O120" s="37"/>
-      <c r="P120" s="37">
-        <v>0</v>
-      </c>
-      <c r="Q120" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
+      <c r="P120" s="37"/>
+      <c r="Q120" s="30"/>
     </row>
     <row r="121" spans="1:17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A121" s="41"/>
@@ -6147,25 +6045,15 @@
       <c r="H121" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="I121" s="37">
-        <v>0</v>
-      </c>
+      <c r="I121" s="37"/>
       <c r="J121" s="37"/>
-      <c r="K121" s="37">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
+      <c r="K121" s="37"/>
       <c r="L121" s="37"/>
       <c r="M121" s="37"/>
       <c r="N121" s="37"/>
       <c r="O121" s="37"/>
-      <c r="P121" s="37">
-        <v>0</v>
-      </c>
-      <c r="Q121" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
+      <c r="P121" s="37"/>
+      <c r="Q121" s="30"/>
     </row>
     <row r="122" spans="1:17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A122" s="31"/>
@@ -6180,25 +6068,15 @@
       <c r="H122" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="I122" s="37">
-        <v>41000</v>
-      </c>
+      <c r="I122" s="37"/>
       <c r="J122" s="37"/>
-      <c r="K122" s="37">
-        <f t="shared" si="9"/>
-        <v>41000</v>
-      </c>
+      <c r="K122" s="37"/>
       <c r="L122" s="37"/>
       <c r="M122" s="37"/>
       <c r="N122" s="37"/>
       <c r="O122" s="37"/>
-      <c r="P122" s="37">
-        <v>41000</v>
-      </c>
-      <c r="Q122" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
+      <c r="P122" s="37"/>
+      <c r="Q122" s="30"/>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A123" s="31"/>
@@ -6456,25 +6334,15 @@
       <c r="H130" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="I130" s="37">
-        <v>310000</v>
-      </c>
+      <c r="I130" s="37"/>
       <c r="J130" s="37"/>
-      <c r="K130" s="37">
-        <f t="shared" si="9"/>
-        <v>310000</v>
-      </c>
+      <c r="K130" s="37"/>
       <c r="L130" s="37"/>
       <c r="M130" s="37"/>
       <c r="N130" s="37"/>
       <c r="O130" s="37"/>
-      <c r="P130" s="37">
-        <v>310000</v>
-      </c>
-      <c r="Q130" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
+      <c r="P130" s="37"/>
+      <c r="Q130" s="30"/>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A131" s="31"/>
@@ -6744,25 +6612,15 @@
       <c r="H138" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="I138" s="37">
-        <v>60500</v>
-      </c>
+      <c r="I138" s="37"/>
       <c r="J138" s="37"/>
-      <c r="K138" s="37">
-        <f t="shared" si="9"/>
-        <v>60500</v>
-      </c>
+      <c r="K138" s="37"/>
       <c r="L138" s="37"/>
       <c r="M138" s="37"/>
       <c r="N138" s="37"/>
       <c r="O138" s="37"/>
-      <c r="P138" s="37">
-        <v>60500</v>
-      </c>
-      <c r="Q138" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
+      <c r="P138" s="37"/>
+      <c r="Q138" s="30"/>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A139" s="31"/>
@@ -7020,25 +6878,15 @@
       <c r="H146" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="I146" s="37">
-        <v>290000</v>
-      </c>
+      <c r="I146" s="37"/>
       <c r="J146" s="37"/>
-      <c r="K146" s="37">
-        <f t="shared" si="9"/>
-        <v>290000</v>
-      </c>
+      <c r="K146" s="37"/>
       <c r="L146" s="37"/>
       <c r="M146" s="37"/>
       <c r="N146" s="37"/>
       <c r="O146" s="37"/>
-      <c r="P146" s="37">
-        <v>290000</v>
-      </c>
-      <c r="Q146" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
+      <c r="P146" s="37"/>
+      <c r="Q146" s="30"/>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A147" s="31"/>
@@ -7318,25 +7166,15 @@
       <c r="H154" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="I154" s="37">
-        <v>116000</v>
-      </c>
+      <c r="I154" s="37"/>
       <c r="J154" s="37"/>
-      <c r="K154" s="37">
-        <f t="shared" si="9"/>
-        <v>116000</v>
-      </c>
+      <c r="K154" s="37"/>
       <c r="L154" s="37"/>
       <c r="M154" s="37"/>
       <c r="N154" s="37"/>
       <c r="O154" s="37"/>
-      <c r="P154" s="37">
-        <v>116000</v>
-      </c>
-      <c r="Q154" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
+      <c r="P154" s="37"/>
+      <c r="Q154" s="30"/>
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A155" s="31"/>
@@ -7602,25 +7440,15 @@
       <c r="H162" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="I162" s="37">
-        <v>46000</v>
-      </c>
+      <c r="I162" s="37"/>
       <c r="J162" s="37"/>
-      <c r="K162" s="37">
-        <f t="shared" si="9"/>
-        <v>46000</v>
-      </c>
+      <c r="K162" s="37"/>
       <c r="L162" s="37"/>
       <c r="M162" s="37"/>
       <c r="N162" s="37"/>
       <c r="O162" s="37"/>
-      <c r="P162" s="37">
-        <v>46000</v>
-      </c>
-      <c r="Q162" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
+      <c r="P162" s="37"/>
+      <c r="Q162" s="30"/>
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A163" s="31"/>
@@ -7866,25 +7694,15 @@
       <c r="H170" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="I170" s="37">
-        <v>18000</v>
-      </c>
+      <c r="I170" s="37"/>
       <c r="J170" s="37"/>
-      <c r="K170" s="37">
-        <f t="shared" si="9"/>
-        <v>18000</v>
-      </c>
+      <c r="K170" s="37"/>
       <c r="L170" s="37"/>
       <c r="M170" s="37"/>
       <c r="N170" s="37"/>
       <c r="O170" s="37"/>
-      <c r="P170" s="37">
-        <v>18000</v>
-      </c>
-      <c r="Q170" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
+      <c r="P170" s="37"/>
+      <c r="Q170" s="30"/>
     </row>
     <row r="171" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A171" s="31"/>
@@ -8052,25 +7870,15 @@
       <c r="H176" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="I176" s="37">
-        <v>0</v>
-      </c>
+      <c r="I176" s="37"/>
       <c r="J176" s="37"/>
-      <c r="K176" s="37">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
+      <c r="K176" s="37"/>
       <c r="L176" s="37"/>
       <c r="M176" s="37"/>
       <c r="N176" s="37"/>
       <c r="O176" s="37"/>
-      <c r="P176" s="37">
-        <v>0</v>
-      </c>
-      <c r="Q176" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
+      <c r="P176" s="37"/>
+      <c r="Q176" s="30"/>
     </row>
     <row r="177" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A177" s="31"/>
@@ -8159,25 +7967,15 @@
       <c r="H179" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="I179" s="37">
-        <v>10500</v>
-      </c>
+      <c r="I179" s="37"/>
       <c r="J179" s="37"/>
-      <c r="K179" s="37">
-        <f t="shared" si="9"/>
-        <v>10500</v>
-      </c>
+      <c r="K179" s="37"/>
       <c r="L179" s="37"/>
       <c r="M179" s="37"/>
       <c r="N179" s="37"/>
       <c r="O179" s="37"/>
-      <c r="P179" s="37">
-        <v>10500</v>
-      </c>
-      <c r="Q179" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
+      <c r="P179" s="37"/>
+      <c r="Q179" s="30"/>
     </row>
     <row r="180" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A180" s="31"/>
@@ -8402,25 +8200,15 @@
       <c r="H186" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="I186" s="37">
-        <v>6000</v>
-      </c>
+      <c r="I186" s="37"/>
       <c r="J186" s="37"/>
-      <c r="K186" s="37">
-        <f t="shared" si="9"/>
-        <v>6000</v>
-      </c>
+      <c r="K186" s="37"/>
       <c r="L186" s="37"/>
       <c r="M186" s="37"/>
       <c r="N186" s="37"/>
       <c r="O186" s="37"/>
-      <c r="P186" s="37">
-        <v>6000</v>
-      </c>
-      <c r="Q186" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
+      <c r="P186" s="37"/>
+      <c r="Q186" s="30"/>
     </row>
     <row r="187" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A187" s="31"/>
@@ -8689,25 +8477,15 @@
       <c r="H195" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="I195" s="37">
-        <v>7400</v>
-      </c>
+      <c r="I195" s="37"/>
       <c r="J195" s="37"/>
-      <c r="K195" s="37">
-        <f t="shared" si="9"/>
-        <v>7400</v>
-      </c>
+      <c r="K195" s="37"/>
       <c r="L195" s="37"/>
       <c r="M195" s="37"/>
       <c r="N195" s="37"/>
       <c r="O195" s="37"/>
-      <c r="P195" s="37">
-        <v>7400</v>
-      </c>
-      <c r="Q195" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
+      <c r="P195" s="37"/>
+      <c r="Q195" s="30"/>
     </row>
     <row r="196" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A196" s="31"/>
@@ -8893,25 +8671,15 @@
       <c r="H201" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="I201" s="37">
-        <v>15000</v>
-      </c>
+      <c r="I201" s="37"/>
       <c r="J201" s="37"/>
-      <c r="K201" s="37">
-        <f t="shared" si="9"/>
-        <v>15000</v>
-      </c>
+      <c r="K201" s="37"/>
       <c r="L201" s="37"/>
       <c r="M201" s="37"/>
       <c r="N201" s="37"/>
       <c r="O201" s="37"/>
-      <c r="P201" s="37">
-        <v>15000</v>
-      </c>
-      <c r="Q201" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
+      <c r="P201" s="37"/>
+      <c r="Q201" s="30"/>
     </row>
     <row r="202" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A202" s="31"/>
@@ -8984,25 +8752,15 @@
       <c r="H204" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="I204" s="37">
-        <v>698500</v>
-      </c>
+      <c r="I204" s="37"/>
       <c r="J204" s="37"/>
-      <c r="K204" s="37">
-        <f t="shared" si="9"/>
-        <v>698500</v>
-      </c>
+      <c r="K204" s="37"/>
       <c r="L204" s="37"/>
       <c r="M204" s="37"/>
       <c r="N204" s="37"/>
       <c r="O204" s="37"/>
-      <c r="P204" s="37">
-        <v>698500</v>
-      </c>
-      <c r="Q204" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
+      <c r="P204" s="37"/>
+      <c r="Q204" s="30"/>
     </row>
     <row r="205" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A205" s="31"/>
@@ -9572,25 +9330,15 @@
       <c r="H220" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="I220" s="37">
-        <v>51000</v>
-      </c>
+      <c r="I220" s="37"/>
       <c r="J220" s="37"/>
-      <c r="K220" s="37">
-        <f t="shared" si="9"/>
-        <v>51000</v>
-      </c>
+      <c r="K220" s="37"/>
       <c r="L220" s="37"/>
       <c r="M220" s="37"/>
       <c r="N220" s="37"/>
       <c r="O220" s="37"/>
-      <c r="P220" s="37">
-        <v>51000</v>
-      </c>
-      <c r="Q220" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
+      <c r="P220" s="37"/>
+      <c r="Q220" s="30"/>
     </row>
     <row r="221" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A221" s="31"/>
@@ -9901,25 +9649,15 @@
       <c r="H229" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="I229" s="37">
-        <v>0</v>
-      </c>
+      <c r="I229" s="37"/>
       <c r="J229" s="37"/>
-      <c r="K229" s="37">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
+      <c r="K229" s="37"/>
       <c r="L229" s="37"/>
       <c r="M229" s="37"/>
       <c r="N229" s="37"/>
       <c r="O229" s="37"/>
-      <c r="P229" s="37">
-        <v>0</v>
-      </c>
-      <c r="Q229" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
+      <c r="P229" s="37"/>
+      <c r="Q229" s="30"/>
     </row>
     <row r="230" spans="1:17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A230" s="38"/>
@@ -9933,39 +9671,39 @@
         <v>43</v>
       </c>
       <c r="I230" s="5">
-        <f t="shared" ref="I230:Q230" si="11">SUM(I87:I229)</f>
-        <v>3666535</v>
+        <f t="shared" ref="I230:Q230" si="6">SUM(I87:I229)</f>
+        <v>1885635</v>
       </c>
       <c r="J230" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K230" s="5">
-        <f t="shared" si="11"/>
-        <v>3666535</v>
+        <f t="shared" si="6"/>
+        <v>1885635</v>
       </c>
       <c r="L230" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>1155614.8999999999</v>
       </c>
       <c r="M230" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>219113.1</v>
       </c>
       <c r="N230" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>1155614.8999999999</v>
       </c>
       <c r="O230" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>107118.33</v>
       </c>
       <c r="P230" s="5">
-        <f t="shared" si="11"/>
-        <v>2388154.5099999998</v>
+        <f t="shared" si="6"/>
+        <v>607254.51000000013</v>
       </c>
       <c r="Q230" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>17241.260000000002</v>
       </c>
     </row>
@@ -9982,38 +9720,38 @@
       </c>
       <c r="I231" s="3">
         <f>I230</f>
-        <v>3666535</v>
+        <v>1885635</v>
       </c>
       <c r="J231" s="3">
-        <f t="shared" ref="J231:Q231" si="12">J230</f>
+        <f t="shared" ref="J231:Q231" si="7">J230</f>
         <v>0</v>
       </c>
       <c r="K231" s="3">
-        <f t="shared" si="12"/>
-        <v>3666535</v>
+        <f t="shared" si="7"/>
+        <v>1885635</v>
       </c>
       <c r="L231" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>1155614.8999999999</v>
       </c>
       <c r="M231" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>219113.1</v>
       </c>
       <c r="N231" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>1155614.8999999999</v>
       </c>
       <c r="O231" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>107118.33</v>
       </c>
       <c r="P231" s="3">
-        <f t="shared" si="12"/>
-        <v>2388154.5099999998</v>
+        <f t="shared" si="7"/>
+        <v>607254.51000000013</v>
       </c>
       <c r="Q231" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>17241.260000000002</v>
       </c>
     </row>
@@ -10076,9 +9814,7 @@
       <c r="H234" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="I234" s="37">
-        <v>53000</v>
-      </c>
+      <c r="I234" s="37"/>
       <c r="J234" s="37"/>
       <c r="K234" s="37"/>
       <c r="L234" s="37"/>
@@ -10148,7 +9884,7 @@
         <v>0</v>
       </c>
       <c r="K237" s="76">
-        <f t="shared" ref="K237" si="13">I237+J237</f>
+        <f t="shared" ref="K237" si="8">I237+J237</f>
         <v>0</v>
       </c>
       <c r="L237" s="76">
@@ -10164,11 +9900,11 @@
         <v>0</v>
       </c>
       <c r="P237" s="76">
-        <f t="shared" ref="P237" si="14">K237-N237-O237</f>
+        <f t="shared" ref="P237" si="9">K237-N237-O237</f>
         <v>0</v>
       </c>
       <c r="Q237" s="76">
-        <f t="shared" ref="Q237" si="15">L237+M237-N237-O237</f>
+        <f t="shared" ref="Q237" si="10">L237+M237-N237-O237</f>
         <v>0</v>
       </c>
     </row>
@@ -10377,9 +10113,7 @@
       <c r="H244" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="I244" s="37">
-        <v>89600</v>
-      </c>
+      <c r="I244" s="37"/>
       <c r="J244" s="37"/>
       <c r="K244" s="37"/>
       <c r="L244" s="37"/>
@@ -10727,9 +10461,7 @@
       <c r="H254" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="I254" s="37">
-        <v>3700</v>
-      </c>
+      <c r="I254" s="37"/>
       <c r="J254" s="37"/>
       <c r="K254" s="37"/>
       <c r="L254" s="37"/>
@@ -11061,9 +10793,7 @@
       <c r="H264" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="I264" s="37">
-        <v>54500</v>
-      </c>
+      <c r="I264" s="37"/>
       <c r="J264" s="37"/>
       <c r="K264" s="37"/>
       <c r="L264" s="37"/>
@@ -11782,9 +11512,7 @@
       <c r="H285" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="I285" s="37">
-        <v>0</v>
-      </c>
+      <c r="I285" s="37"/>
       <c r="J285" s="37"/>
       <c r="K285" s="37"/>
       <c r="L285" s="37"/>
@@ -12044,9 +11772,7 @@
       <c r="H293" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="I293" s="37">
-        <v>59000</v>
-      </c>
+      <c r="I293" s="37"/>
       <c r="J293" s="37"/>
       <c r="K293" s="37"/>
       <c r="L293" s="37"/>
@@ -12394,9 +12120,7 @@
       <c r="H303" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="I303" s="37">
-        <v>221200</v>
-      </c>
+      <c r="I303" s="37"/>
       <c r="J303" s="37"/>
       <c r="K303" s="37"/>
       <c r="L303" s="37"/>
@@ -12746,9 +12470,7 @@
       <c r="H313" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="I313" s="37">
-        <v>52500</v>
-      </c>
+      <c r="I313" s="37"/>
       <c r="J313" s="37"/>
       <c r="K313" s="37"/>
       <c r="L313" s="37"/>
@@ -13100,9 +12822,7 @@
       <c r="H323" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="I323" s="37">
-        <v>210500</v>
-      </c>
+      <c r="I323" s="37"/>
       <c r="J323" s="37"/>
       <c r="K323" s="37"/>
       <c r="L323" s="37"/>
@@ -13456,9 +13176,7 @@
       <c r="H333" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="I333" s="37">
-        <v>92000</v>
-      </c>
+      <c r="I333" s="37"/>
       <c r="J333" s="37"/>
       <c r="K333" s="37"/>
       <c r="L333" s="37"/>
@@ -13810,9 +13528,7 @@
       <c r="H343" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="I343" s="37">
-        <v>42000</v>
-      </c>
+      <c r="I343" s="37"/>
       <c r="J343" s="37"/>
       <c r="K343" s="37"/>
       <c r="L343" s="37"/>
@@ -14162,9 +13878,7 @@
       <c r="H353" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="I353" s="37">
-        <v>52000</v>
-      </c>
+      <c r="I353" s="37"/>
       <c r="J353" s="37"/>
       <c r="K353" s="37"/>
       <c r="L353" s="37"/>
@@ -14518,9 +14232,7 @@
       <c r="H363" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="I363" s="37">
-        <v>0</v>
-      </c>
+      <c r="I363" s="37"/>
       <c r="J363" s="37"/>
       <c r="K363" s="37"/>
       <c r="L363" s="37"/>
@@ -14780,9 +14492,7 @@
       <c r="H371" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="I371" s="37">
-        <v>4500</v>
-      </c>
+      <c r="I371" s="37"/>
       <c r="J371" s="37"/>
       <c r="K371" s="37"/>
       <c r="L371" s="37"/>
@@ -15097,9 +14807,7 @@
       <c r="H380" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="I380" s="37">
-        <v>9000</v>
-      </c>
+      <c r="I380" s="37"/>
       <c r="J380" s="37"/>
       <c r="K380" s="37"/>
       <c r="L380" s="37"/>
@@ -15447,9 +15155,7 @@
       <c r="H390" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="I390" s="37">
-        <v>1000</v>
-      </c>
+      <c r="I390" s="37"/>
       <c r="J390" s="37"/>
       <c r="K390" s="37"/>
       <c r="L390" s="37"/>
@@ -15701,9 +15407,7 @@
       <c r="H398" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="I398" s="37">
-        <v>45000</v>
-      </c>
+      <c r="I398" s="37"/>
       <c r="J398" s="37"/>
       <c r="K398" s="37"/>
       <c r="L398" s="37"/>
@@ -16041,9 +15745,7 @@
       <c r="H408" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="I408" s="37">
-        <v>383500</v>
-      </c>
+      <c r="I408" s="37"/>
       <c r="J408" s="37"/>
       <c r="K408" s="37"/>
       <c r="L408" s="37"/>
@@ -16510,9 +16212,7 @@
       <c r="H421" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="I421" s="37">
-        <v>90000</v>
-      </c>
+      <c r="I421" s="37"/>
       <c r="J421" s="37"/>
       <c r="K421" s="37"/>
       <c r="L421" s="37"/>
@@ -16934,9 +16634,7 @@
       <c r="H433" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="I433" s="37">
-        <v>0</v>
-      </c>
+      <c r="I433" s="37"/>
       <c r="J433" s="37"/>
       <c r="K433" s="37"/>
       <c r="L433" s="37"/>
@@ -17196,7 +16894,7 @@
       </c>
       <c r="I441" s="5">
         <f>SUM(I234:I433)</f>
-        <v>2995200</v>
+        <v>1532200</v>
       </c>
       <c r="J441" s="5"/>
       <c r="K441" s="5"/>
@@ -17220,7 +16918,7 @@
       </c>
       <c r="I442" s="3">
         <f>I441</f>
-        <v>2995200</v>
+        <v>1532200</v>
       </c>
       <c r="J442" s="3"/>
       <c r="K442" s="3"/>
@@ -17738,9 +17436,7 @@
       <c r="H464" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="I464" s="37">
-        <v>236200</v>
-      </c>
+      <c r="I464" s="37"/>
       <c r="J464" s="37"/>
       <c r="K464" s="37"/>
       <c r="L464" s="37"/>
@@ -17868,7 +17564,7 @@
       </c>
       <c r="I468" s="5">
         <f>SUM(I464)</f>
-        <v>236200</v>
+        <v>0</v>
       </c>
       <c r="J468" s="5"/>
       <c r="K468" s="5"/>
@@ -17892,7 +17588,7 @@
       </c>
       <c r="I469" s="3">
         <f>I468</f>
-        <v>236200</v>
+        <v>0</v>
       </c>
       <c r="J469" s="3"/>
       <c r="K469" s="3"/>
@@ -17962,9 +17658,7 @@
       <c r="H472" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="I472" s="37">
-        <v>244000</v>
-      </c>
+      <c r="I472" s="37"/>
       <c r="J472" s="37"/>
       <c r="K472" s="37"/>
       <c r="L472" s="37"/>
@@ -17992,7 +17686,7 @@
         <v>0</v>
       </c>
       <c r="K473" s="76">
-        <f t="shared" ref="K473" si="16">I473+J473</f>
+        <f t="shared" ref="K473" si="11">I473+J473</f>
         <v>5000</v>
       </c>
       <c r="L473" s="76">
@@ -18008,11 +17702,11 @@
         <v>0</v>
       </c>
       <c r="P473" s="76">
-        <f t="shared" ref="P473" si="17">K473-N473-O473</f>
+        <f t="shared" ref="P473" si="12">K473-N473-O473</f>
         <v>5000</v>
       </c>
       <c r="Q473" s="76">
-        <f t="shared" ref="Q473" si="18">L473+M473-N473-O473</f>
+        <f t="shared" ref="Q473" si="13">L473+M473-N473-O473</f>
         <v>0</v>
       </c>
     </row>
@@ -18107,7 +17801,7 @@
       </c>
       <c r="I476" s="5">
         <f>SUM(I472)</f>
-        <v>244000</v>
+        <v>0</v>
       </c>
       <c r="J476" s="5"/>
       <c r="K476" s="5"/>
@@ -18131,7 +17825,7 @@
       </c>
       <c r="I477" s="3">
         <f>I476</f>
-        <v>244000</v>
+        <v>0</v>
       </c>
       <c r="J477" s="3"/>
       <c r="K477" s="3"/>
@@ -18201,9 +17895,7 @@
       <c r="H480" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="I480" s="37">
-        <v>0</v>
-      </c>
+      <c r="I480" s="37"/>
       <c r="J480" s="37"/>
       <c r="K480" s="37"/>
       <c r="L480" s="37"/>
@@ -18226,9 +17918,7 @@
       <c r="H481" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="I481" s="37">
-        <v>91700</v>
-      </c>
+      <c r="I481" s="37"/>
       <c r="J481" s="37"/>
       <c r="K481" s="37"/>
       <c r="L481" s="37"/>
@@ -18545,9 +18235,7 @@
       <c r="H490" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="I490" s="37">
-        <v>16800</v>
-      </c>
+      <c r="I490" s="37"/>
       <c r="J490" s="37"/>
       <c r="K490" s="37"/>
       <c r="L490" s="37"/>
@@ -18749,9 +18437,7 @@
       <c r="H496" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="I496" s="37">
-        <v>50800</v>
-      </c>
+      <c r="I496" s="37"/>
       <c r="J496" s="37"/>
       <c r="K496" s="37"/>
       <c r="L496" s="37"/>
@@ -18873,9 +18559,7 @@
       <c r="H500" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="I500" s="37">
-        <v>571000</v>
-      </c>
+      <c r="I500" s="37"/>
       <c r="J500" s="37"/>
       <c r="K500" s="37"/>
       <c r="L500" s="37"/>
@@ -19081,9 +18765,7 @@
       <c r="H506" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="I506" s="37">
-        <v>32800</v>
-      </c>
+      <c r="I506" s="37"/>
       <c r="J506" s="37"/>
       <c r="K506" s="37"/>
       <c r="L506" s="37"/>
@@ -19320,9 +19002,7 @@
       <c r="H513" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="I513" s="37">
-        <v>57000</v>
-      </c>
+      <c r="I513" s="37"/>
       <c r="J513" s="37"/>
       <c r="K513" s="37"/>
       <c r="L513" s="37"/>
@@ -19639,7 +19319,7 @@
       </c>
       <c r="I522" s="5">
         <f>SUM(I480:I513)</f>
-        <v>1344200</v>
+        <v>524100</v>
       </c>
       <c r="J522" s="5"/>
       <c r="K522" s="5"/>
@@ -19686,9 +19366,7 @@
       <c r="H524" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="I524" s="37">
-        <v>48000</v>
-      </c>
+      <c r="I524" s="37"/>
       <c r="J524" s="37"/>
       <c r="K524" s="37"/>
       <c r="L524" s="37"/>
@@ -19789,9 +19467,7 @@
       <c r="H527" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="I527" s="37">
-        <v>28000</v>
-      </c>
+      <c r="I527" s="37"/>
       <c r="J527" s="37"/>
       <c r="K527" s="37"/>
       <c r="L527" s="37"/>
@@ -20065,9 +19741,7 @@
       <c r="H535" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="I535" s="37">
-        <v>30000</v>
-      </c>
+      <c r="I535" s="37"/>
       <c r="J535" s="37"/>
       <c r="K535" s="37"/>
       <c r="L535" s="37"/>
@@ -20388,9 +20062,7 @@
       <c r="H544" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="I544" s="37">
-        <v>8500</v>
-      </c>
+      <c r="I544" s="37"/>
       <c r="J544" s="37"/>
       <c r="K544" s="37"/>
       <c r="L544" s="37"/>
@@ -20590,9 +20262,7 @@
       <c r="H550" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="I550" s="37">
-        <v>15500</v>
-      </c>
+      <c r="I550" s="37"/>
       <c r="J550" s="37"/>
       <c r="K550" s="37"/>
       <c r="L550" s="37"/>
@@ -20909,9 +20579,7 @@
       <c r="H559" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="I559" s="37">
-        <v>15000</v>
-      </c>
+      <c r="I559" s="37"/>
       <c r="J559" s="37"/>
       <c r="K559" s="37"/>
       <c r="L559" s="37"/>
@@ -21267,7 +20935,7 @@
       </c>
       <c r="I569" s="5">
         <f>SUM(I524:I559)</f>
-        <v>230950</v>
+        <v>85950</v>
       </c>
       <c r="J569" s="5"/>
       <c r="K569" s="5"/>
@@ -21291,7 +20959,7 @@
       </c>
       <c r="I570" s="3">
         <f>I569+I522</f>
-        <v>1575150</v>
+        <v>610050</v>
       </c>
       <c r="J570" s="3"/>
       <c r="K570" s="3"/>
@@ -21361,9 +21029,7 @@
       <c r="H573" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="I573" s="37">
-        <v>0</v>
-      </c>
+      <c r="I573" s="37"/>
       <c r="J573" s="37"/>
       <c r="K573" s="37"/>
       <c r="L573" s="37"/>
@@ -21503,9 +21169,7 @@
       <c r="H577" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="I577" s="37">
-        <v>84000</v>
-      </c>
+      <c r="I577" s="37"/>
       <c r="J577" s="37"/>
       <c r="K577" s="37"/>
       <c r="L577" s="37"/>
@@ -21822,9 +21486,7 @@
       <c r="H586" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="I586" s="37">
-        <v>25000</v>
-      </c>
+      <c r="I586" s="37"/>
       <c r="J586" s="37"/>
       <c r="K586" s="37"/>
       <c r="L586" s="37"/>
@@ -22036,9 +21698,7 @@
       <c r="H592" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="I592" s="37">
-        <v>516000</v>
-      </c>
+      <c r="I592" s="37"/>
       <c r="J592" s="37"/>
       <c r="K592" s="37"/>
       <c r="L592" s="37"/>
@@ -22256,9 +21916,7 @@
       <c r="H598" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="I598" s="37">
-        <v>993000</v>
-      </c>
+      <c r="I598" s="37"/>
       <c r="J598" s="37"/>
       <c r="K598" s="37"/>
       <c r="L598" s="37"/>
@@ -22398,9 +22056,7 @@
       <c r="H602" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="I602" s="37">
-        <v>40000</v>
-      </c>
+      <c r="I602" s="37"/>
       <c r="J602" s="37"/>
       <c r="K602" s="37"/>
       <c r="L602" s="37"/>
@@ -22682,9 +22338,7 @@
       <c r="H610" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="I610" s="37">
-        <v>107000</v>
-      </c>
+      <c r="I610" s="37"/>
       <c r="J610" s="37"/>
       <c r="K610" s="37"/>
       <c r="L610" s="37"/>
@@ -22972,7 +22626,7 @@
       </c>
       <c r="I618" s="5">
         <f>SUM(I573:I610)</f>
-        <v>2493720</v>
+        <v>728720</v>
       </c>
       <c r="J618" s="5"/>
       <c r="K618" s="5"/>
@@ -23019,9 +22673,7 @@
       <c r="H620" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="I620" s="37">
-        <v>3000</v>
-      </c>
+      <c r="I620" s="37"/>
       <c r="J620" s="37"/>
       <c r="K620" s="37"/>
       <c r="L620" s="37"/>
@@ -23229,9 +22881,7 @@
       <c r="H626" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="I626" s="37">
-        <v>22000</v>
-      </c>
+      <c r="I626" s="37"/>
       <c r="J626" s="37"/>
       <c r="K626" s="37"/>
       <c r="L626" s="37"/>
@@ -23507,9 +23157,7 @@
       <c r="H634" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="I634" s="37">
-        <v>16500</v>
-      </c>
+      <c r="I634" s="37"/>
       <c r="J634" s="37"/>
       <c r="K634" s="37"/>
       <c r="L634" s="37"/>
@@ -23795,9 +23443,7 @@
       <c r="H642" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="I642" s="37">
-        <v>2000</v>
-      </c>
+      <c r="I642" s="37"/>
       <c r="J642" s="37"/>
       <c r="K642" s="37"/>
       <c r="L642" s="37"/>
@@ -23976,9 +23622,7 @@
       <c r="H647" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="I647" s="37">
-        <v>11500</v>
-      </c>
+      <c r="I647" s="37"/>
       <c r="J647" s="37"/>
       <c r="K647" s="37"/>
       <c r="L647" s="37"/>
@@ -24258,9 +23902,7 @@
       <c r="H655" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="I655" s="37">
-        <v>10500</v>
-      </c>
+      <c r="I655" s="37"/>
       <c r="J655" s="37"/>
       <c r="K655" s="37"/>
       <c r="L655" s="37"/>
@@ -24538,7 +24180,7 @@
       </c>
       <c r="I663" s="5">
         <f>SUM(I620:I655)</f>
-        <v>120500</v>
+        <v>55000</v>
       </c>
       <c r="J663" s="5"/>
       <c r="K663" s="5"/>
@@ -24562,7 +24204,7 @@
       </c>
       <c r="I664" s="3">
         <f>I618+I663</f>
-        <v>2614220</v>
+        <v>783720</v>
       </c>
       <c r="J664" s="3"/>
       <c r="K664" s="3"/>
@@ -24632,9 +24274,7 @@
       <c r="H667" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="I667" s="37">
-        <v>939100</v>
-      </c>
+      <c r="I667" s="37"/>
       <c r="J667" s="37"/>
       <c r="K667" s="37"/>
       <c r="L667" s="37"/>
@@ -24840,9 +24480,7 @@
       <c r="H673" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="I673" s="37">
-        <v>40300</v>
-      </c>
+      <c r="I673" s="37"/>
       <c r="J673" s="37"/>
       <c r="K673" s="37"/>
       <c r="L673" s="37"/>
@@ -24900,9 +24538,7 @@
       <c r="H675" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="I675" s="37">
-        <v>273200</v>
-      </c>
+      <c r="I675" s="37"/>
       <c r="J675" s="37"/>
       <c r="K675" s="37"/>
       <c r="L675" s="37"/>
@@ -25032,9 +24668,7 @@
       <c r="H679" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="I679" s="37">
-        <v>1241000</v>
-      </c>
+      <c r="I679" s="37"/>
       <c r="J679" s="37"/>
       <c r="K679" s="37"/>
       <c r="L679" s="37"/>
@@ -25096,7 +24730,7 @@
       </c>
       <c r="I681" s="5">
         <f>SUM(I667:I679)</f>
-        <v>3754200</v>
+        <v>1260600</v>
       </c>
       <c r="J681" s="5"/>
       <c r="K681" s="5"/>
@@ -25143,9 +24777,7 @@
       <c r="H683" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="I683" s="37">
-        <v>160000</v>
-      </c>
+      <c r="I683" s="37"/>
       <c r="J683" s="37"/>
       <c r="K683" s="37"/>
       <c r="L683" s="37"/>
@@ -25286,9 +24918,7 @@
       <c r="H688" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="I688" s="37">
-        <v>76000</v>
-      </c>
+      <c r="I688" s="37"/>
       <c r="J688" s="37"/>
       <c r="K688" s="37"/>
       <c r="L688" s="37"/>
@@ -25503,9 +25133,7 @@
       <c r="H695" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="I695" s="37">
-        <v>0</v>
-      </c>
+      <c r="I695" s="37"/>
       <c r="J695" s="37"/>
       <c r="K695" s="37"/>
       <c r="L695" s="37"/>
@@ -25528,7 +25156,7 @@
       </c>
       <c r="I696" s="5">
         <f>SUM(I683:I695)</f>
-        <v>472000</v>
+        <v>236000</v>
       </c>
       <c r="J696" s="5"/>
       <c r="K696" s="5"/>
@@ -25575,9 +25203,7 @@
       <c r="H698" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="I698" s="37">
-        <v>415000</v>
-      </c>
+      <c r="I698" s="37"/>
       <c r="J698" s="37"/>
       <c r="K698" s="37"/>
       <c r="L698" s="37"/>
@@ -25831,9 +25457,7 @@
       <c r="H706" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="I706" s="37">
-        <v>1000000</v>
-      </c>
+      <c r="I706" s="37"/>
       <c r="J706" s="37"/>
       <c r="K706" s="37"/>
       <c r="L706" s="37"/>
@@ -26087,7 +25711,7 @@
       </c>
       <c r="I714" s="5">
         <f>SUM(I698:I706)</f>
-        <v>1830000</v>
+        <v>415000</v>
       </c>
       <c r="J714" s="5"/>
       <c r="K714" s="5"/>
@@ -26111,7 +25735,7 @@
       </c>
       <c r="I715" s="3">
         <f>I681+I696+I714</f>
-        <v>6056200</v>
+        <v>1911600</v>
       </c>
       <c r="J715" s="3"/>
       <c r="K715" s="3"/>
@@ -27712,9 +27336,7 @@
       <c r="H763" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="I763" s="37">
-        <v>305000</v>
-      </c>
+      <c r="I763" s="37"/>
       <c r="J763" s="37"/>
       <c r="K763" s="37"/>
       <c r="L763" s="37"/>
@@ -27982,9 +27604,7 @@
       <c r="H771" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="I771" s="37">
-        <v>1700000</v>
-      </c>
+      <c r="I771" s="37"/>
       <c r="J771" s="37"/>
       <c r="K771" s="37"/>
       <c r="L771" s="37"/>
@@ -28285,7 +27905,7 @@
       </c>
       <c r="I780" s="5">
         <f>SUM(I763:I771)</f>
-        <v>2310000</v>
+        <v>305000</v>
       </c>
       <c r="J780" s="5"/>
       <c r="K780" s="5"/>
@@ -28309,7 +27929,7 @@
       </c>
       <c r="I781" s="3">
         <f>I741+I761+I780</f>
-        <v>3379095.24</v>
+        <v>1374095.24</v>
       </c>
       <c r="J781" s="3"/>
       <c r="K781" s="3"/>
@@ -28379,9 +27999,7 @@
       <c r="H784" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="I784" s="37">
-        <v>0</v>
-      </c>
+      <c r="I784" s="37"/>
       <c r="J784" s="37"/>
       <c r="K784" s="37"/>
       <c r="L784" s="37"/>
@@ -28404,9 +28022,7 @@
       <c r="H785" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="I785" s="37">
-        <v>60000</v>
-      </c>
+      <c r="I785" s="37"/>
       <c r="J785" s="37"/>
       <c r="K785" s="37"/>
       <c r="L785" s="37"/>
@@ -28468,7 +28084,7 @@
       </c>
       <c r="I787" s="5">
         <f>SUM(I784:I785)</f>
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="J787" s="5"/>
       <c r="K787" s="5"/>
@@ -28515,9 +28131,7 @@
       <c r="H789" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="I789" s="37">
-        <v>89100</v>
-      </c>
+      <c r="I789" s="37"/>
       <c r="J789" s="37"/>
       <c r="K789" s="37"/>
       <c r="L789" s="37"/>
@@ -28657,9 +28271,7 @@
       <c r="H793" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="I793" s="37">
-        <v>0</v>
-      </c>
+      <c r="I793" s="37"/>
       <c r="J793" s="37"/>
       <c r="K793" s="37"/>
       <c r="L793" s="37"/>
@@ -28721,7 +28333,7 @@
       </c>
       <c r="I795" s="5">
         <f>SUM(I789:I793)</f>
-        <v>177500</v>
+        <v>88400</v>
       </c>
       <c r="J795" s="5"/>
       <c r="K795" s="5"/>
@@ -28745,7 +28357,7 @@
       </c>
       <c r="I796" s="3">
         <f>I787+I795</f>
-        <v>237500</v>
+        <v>88400</v>
       </c>
       <c r="J796" s="3"/>
       <c r="K796" s="3"/>
@@ -28815,9 +28427,7 @@
       <c r="H799" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="I799" s="37">
-        <v>0</v>
-      </c>
+      <c r="I799" s="37"/>
       <c r="J799" s="37"/>
       <c r="K799" s="37"/>
       <c r="L799" s="37"/>
@@ -28840,9 +28450,7 @@
       <c r="H800" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="I800" s="37">
-        <v>0</v>
-      </c>
+      <c r="I800" s="37"/>
       <c r="J800" s="37"/>
       <c r="K800" s="37"/>
       <c r="L800" s="37"/>
@@ -28911,9 +28519,7 @@
       <c r="H803" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="I803" s="37">
-        <v>24200</v>
-      </c>
+      <c r="I803" s="37"/>
       <c r="J803" s="37"/>
       <c r="K803" s="37"/>
       <c r="L803" s="37"/>
@@ -29123,9 +28729,7 @@
       <c r="H809" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="I809" s="37">
-        <v>0</v>
-      </c>
+      <c r="I809" s="37"/>
       <c r="J809" s="37"/>
       <c r="K809" s="37"/>
       <c r="L809" s="37"/>
@@ -29358,9 +28962,7 @@
       <c r="H817" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="I817" s="37">
-        <v>0</v>
-      </c>
+      <c r="I817" s="37"/>
       <c r="J817" s="37"/>
       <c r="K817" s="37"/>
       <c r="L817" s="37"/>
@@ -29476,9 +29078,7 @@
       <c r="H822" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="I822" s="37">
-        <v>0</v>
-      </c>
+      <c r="I822" s="37"/>
       <c r="J822" s="37"/>
       <c r="K822" s="37"/>
       <c r="L822" s="37"/>
@@ -29594,9 +29194,7 @@
       <c r="H827" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="I827" s="37">
-        <v>2347000</v>
-      </c>
+      <c r="I827" s="37"/>
       <c r="J827" s="37"/>
       <c r="K827" s="37"/>
       <c r="L827" s="37"/>
@@ -29864,9 +29462,7 @@
       <c r="H835" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="I835" s="37">
-        <v>105000</v>
-      </c>
+      <c r="I835" s="37"/>
       <c r="J835" s="37"/>
       <c r="K835" s="37"/>
       <c r="L835" s="37"/>
@@ -29961,9 +29557,7 @@
       <c r="H838" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="I838" s="37">
-        <v>368000</v>
-      </c>
+      <c r="I838" s="37"/>
       <c r="J838" s="37"/>
       <c r="K838" s="37"/>
       <c r="L838" s="37"/>
@@ -30134,9 +29728,7 @@
       <c r="H843" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="I843" s="37">
-        <v>224400</v>
-      </c>
+      <c r="I843" s="37"/>
       <c r="J843" s="37"/>
       <c r="K843" s="37"/>
       <c r="L843" s="37"/>
@@ -30336,9 +29928,7 @@
       <c r="H849" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="I849" s="37">
-        <v>280000</v>
-      </c>
+      <c r="I849" s="37"/>
       <c r="J849" s="37"/>
       <c r="K849" s="37"/>
       <c r="L849" s="37"/>
@@ -30567,9 +30157,7 @@
       <c r="H856" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="I856" s="37">
-        <v>20000</v>
-      </c>
+      <c r="I856" s="37"/>
       <c r="J856" s="37"/>
       <c r="K856" s="37"/>
       <c r="L856" s="37"/>
@@ -30631,9 +30219,7 @@
       <c r="H858" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="I858" s="37">
-        <v>142000</v>
-      </c>
+      <c r="I858" s="37"/>
       <c r="J858" s="37"/>
       <c r="K858" s="37"/>
       <c r="L858" s="37"/>
@@ -30885,9 +30471,7 @@
       <c r="H866" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="I866" s="37">
-        <v>225000</v>
-      </c>
+      <c r="I866" s="37"/>
       <c r="J866" s="37"/>
       <c r="K866" s="37"/>
       <c r="L866" s="37"/>
@@ -30949,9 +30533,7 @@
       <c r="H868" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="I868" s="37">
-        <v>35500</v>
-      </c>
+      <c r="I868" s="37"/>
       <c r="J868" s="37"/>
       <c r="K868" s="37"/>
       <c r="L868" s="37"/>
@@ -31176,9 +30758,7 @@
       <c r="H875" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="I875" s="37">
-        <v>115500</v>
-      </c>
+      <c r="I875" s="37"/>
       <c r="J875" s="37"/>
       <c r="K875" s="37"/>
       <c r="L875" s="37"/>
@@ -31405,9 +30985,7 @@
       <c r="H882" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="I882" s="37">
-        <v>34000</v>
-      </c>
+      <c r="I882" s="37"/>
       <c r="J882" s="37"/>
       <c r="K882" s="37"/>
       <c r="L882" s="37"/>
@@ -31599,9 +31177,7 @@
       <c r="H888" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="I888" s="37">
-        <v>1500</v>
-      </c>
+      <c r="I888" s="37"/>
       <c r="J888" s="37"/>
       <c r="K888" s="37"/>
       <c r="L888" s="37"/>
@@ -31663,9 +31239,7 @@
       <c r="H890" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="I890" s="37">
-        <v>13000</v>
-      </c>
+      <c r="I890" s="37"/>
       <c r="J890" s="37"/>
       <c r="K890" s="37"/>
       <c r="L890" s="37"/>
@@ -31754,9 +31328,7 @@
       <c r="H893" s="46" t="s">
         <v>135</v>
       </c>
-      <c r="I893" s="37">
-        <v>0</v>
-      </c>
+      <c r="I893" s="37"/>
       <c r="J893" s="37"/>
       <c r="K893" s="37"/>
       <c r="L893" s="37"/>
@@ -31779,7 +31351,7 @@
       </c>
       <c r="I894" s="5">
         <f>SUM(I827:I893)</f>
-        <v>7781800</v>
+        <v>3870900</v>
       </c>
       <c r="J894" s="5"/>
       <c r="K894" s="5"/>
@@ -31803,7 +31375,7 @@
       </c>
       <c r="I895" s="3">
         <f>I894</f>
-        <v>7781800</v>
+        <v>3870900</v>
       </c>
       <c r="J895" s="3"/>
       <c r="K895" s="3"/>
@@ -31873,9 +31445,7 @@
       <c r="H898" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="I898" s="37">
-        <v>5810000</v>
-      </c>
+      <c r="I898" s="37"/>
       <c r="J898" s="37"/>
       <c r="K898" s="37"/>
       <c r="L898" s="37"/>
@@ -32085,9 +31655,7 @@
       <c r="H904" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="I904" s="37">
-        <v>65000</v>
-      </c>
+      <c r="I904" s="37"/>
       <c r="J904" s="37"/>
       <c r="K904" s="37"/>
       <c r="L904" s="37"/>
@@ -32215,9 +31783,7 @@
       <c r="H908" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="I908" s="37">
-        <v>553000</v>
-      </c>
+      <c r="I908" s="37"/>
       <c r="J908" s="37"/>
       <c r="K908" s="37"/>
       <c r="L908" s="37"/>
@@ -32384,9 +31950,7 @@
       <c r="H913" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="I913" s="37">
-        <v>390000</v>
-      </c>
+      <c r="I913" s="37"/>
       <c r="J913" s="37"/>
       <c r="K913" s="37"/>
       <c r="L913" s="37"/>
@@ -32514,9 +32078,7 @@
       <c r="H917" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="I917" s="37">
-        <v>455000</v>
-      </c>
+      <c r="I917" s="37"/>
       <c r="J917" s="37"/>
       <c r="K917" s="37"/>
       <c r="L917" s="37"/>
@@ -32730,9 +32292,7 @@
       <c r="H923" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="I923" s="37">
-        <v>240000</v>
-      </c>
+      <c r="I923" s="37"/>
       <c r="J923" s="37"/>
       <c r="K923" s="37"/>
       <c r="L923" s="37"/>
@@ -32860,9 +32420,7 @@
       <c r="H927" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="I927" s="37">
-        <v>225000</v>
-      </c>
+      <c r="I927" s="37"/>
       <c r="J927" s="37"/>
       <c r="K927" s="37"/>
       <c r="L927" s="37"/>
@@ -33068,9 +32626,7 @@
       <c r="H933" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="I933" s="37">
-        <v>583000</v>
-      </c>
+      <c r="I933" s="37"/>
       <c r="J933" s="37"/>
       <c r="K933" s="37"/>
       <c r="L933" s="37"/>
@@ -33188,9 +32744,7 @@
       <c r="H937" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="I937" s="37">
-        <v>62000</v>
-      </c>
+      <c r="I937" s="37"/>
       <c r="J937" s="37"/>
       <c r="K937" s="37"/>
       <c r="L937" s="37"/>
@@ -33386,9 +32940,7 @@
       <c r="H943" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="I943" s="37">
-        <v>285000</v>
-      </c>
+      <c r="I943" s="37"/>
       <c r="J943" s="37"/>
       <c r="K943" s="37"/>
       <c r="L943" s="37"/>
@@ -33516,9 +33068,7 @@
       <c r="H947" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="I947" s="37">
-        <v>113000</v>
-      </c>
+      <c r="I947" s="37"/>
       <c r="J947" s="37"/>
       <c r="K947" s="37"/>
       <c r="L947" s="37"/>
@@ -33685,9 +33235,7 @@
       <c r="H952" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="I952" s="37">
-        <v>0</v>
-      </c>
+      <c r="I952" s="37"/>
       <c r="J952" s="37"/>
       <c r="K952" s="37"/>
       <c r="L952" s="37"/>
@@ -33776,9 +33324,7 @@
       <c r="H955" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="I955" s="37">
-        <v>10000</v>
-      </c>
+      <c r="I955" s="37"/>
       <c r="J955" s="37"/>
       <c r="K955" s="37"/>
       <c r="L955" s="37"/>
@@ -33912,9 +33458,7 @@
       <c r="H959" s="46" t="s">
         <v>135</v>
       </c>
-      <c r="I959" s="37">
-        <v>0</v>
-      </c>
+      <c r="I959" s="37"/>
       <c r="J959" s="37"/>
       <c r="K959" s="37"/>
       <c r="L959" s="37"/>
@@ -34009,7 +33553,7 @@
       </c>
       <c r="I962" s="5">
         <f>SUM(I898:I959)</f>
-        <v>16418900</v>
+        <v>7627900</v>
       </c>
       <c r="J962" s="5"/>
       <c r="K962" s="5"/>
@@ -34033,7 +33577,7 @@
       </c>
       <c r="I963" s="3">
         <f>I962</f>
-        <v>16418900</v>
+        <v>7627900</v>
       </c>
       <c r="J963" s="3"/>
       <c r="K963" s="3"/>
@@ -34101,9 +33645,7 @@
       <c r="H966" s="46" t="s">
         <v>141</v>
       </c>
-      <c r="I966" s="37">
-        <v>1393000</v>
-      </c>
+      <c r="I966" s="37"/>
       <c r="J966" s="37"/>
       <c r="K966" s="37"/>
       <c r="L966" s="37"/>
@@ -34367,9 +33909,7 @@
       <c r="H974" s="46" t="s">
         <v>142</v>
       </c>
-      <c r="I974" s="37">
-        <v>261000</v>
-      </c>
+      <c r="I974" s="37"/>
       <c r="J974" s="37"/>
       <c r="K974" s="37"/>
       <c r="L974" s="37"/>
@@ -34598,9 +34138,7 @@
       <c r="H981" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="I981" s="37">
-        <v>0</v>
-      </c>
+      <c r="I981" s="37"/>
       <c r="J981" s="37"/>
       <c r="K981" s="37"/>
       <c r="L981" s="37"/>
@@ -34621,9 +34159,7 @@
       <c r="H982" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="I982" s="37">
-        <v>3600</v>
-      </c>
+      <c r="I982" s="37"/>
       <c r="J982" s="37"/>
       <c r="K982" s="37"/>
       <c r="L982" s="37"/>
@@ -34679,9 +34215,7 @@
       <c r="H984" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="I984" s="37">
-        <v>43800</v>
-      </c>
+      <c r="I984" s="37"/>
       <c r="J984" s="37"/>
       <c r="K984" s="37"/>
       <c r="L984" s="37"/>
@@ -34768,9 +34302,7 @@
       <c r="H987" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="I987" s="37">
-        <v>343200</v>
-      </c>
+      <c r="I987" s="37"/>
       <c r="J987" s="37"/>
       <c r="K987" s="37"/>
       <c r="L987" s="37"/>
@@ -34859,9 +34391,7 @@
       <c r="H990" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="I990" s="37">
-        <v>342000</v>
-      </c>
+      <c r="I990" s="37"/>
       <c r="J990" s="37"/>
       <c r="K990" s="37"/>
       <c r="L990" s="37"/>
@@ -35137,9 +34667,7 @@
       <c r="H998" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="I998" s="37">
-        <v>151000</v>
-      </c>
+      <c r="I998" s="37"/>
       <c r="J998" s="37"/>
       <c r="K998" s="37"/>
       <c r="L998" s="37"/>
@@ -35366,9 +34894,7 @@
       <c r="H1005" s="46" t="s">
         <v>148</v>
       </c>
-      <c r="I1005" s="37">
-        <v>5000</v>
-      </c>
+      <c r="I1005" s="37"/>
       <c r="J1005" s="37"/>
       <c r="K1005" s="37"/>
       <c r="L1005" s="37"/>
@@ -35418,9 +34944,7 @@
       <c r="H1007" s="46" t="s">
         <v>149</v>
       </c>
-      <c r="I1007" s="37">
-        <v>0</v>
-      </c>
+      <c r="I1007" s="37"/>
       <c r="J1007" s="37"/>
       <c r="K1007" s="37"/>
       <c r="L1007" s="37"/>
@@ -35441,9 +34965,7 @@
       <c r="H1008" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="I1008" s="37">
-        <v>0</v>
-      </c>
+      <c r="I1008" s="37"/>
       <c r="J1008" s="37"/>
       <c r="K1008" s="37"/>
       <c r="L1008" s="37"/>
@@ -35464,9 +34986,7 @@
       <c r="H1009" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="I1009" s="37">
-        <v>5000</v>
-      </c>
+      <c r="I1009" s="37"/>
       <c r="J1009" s="37"/>
       <c r="K1009" s="37"/>
       <c r="L1009" s="37"/>
@@ -35516,9 +35036,7 @@
       <c r="H1011" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="I1011" s="37">
-        <v>50000</v>
-      </c>
+      <c r="I1011" s="37"/>
       <c r="J1011" s="37"/>
       <c r="K1011" s="37"/>
       <c r="L1011" s="37"/>
@@ -35574,9 +35092,7 @@
       <c r="H1013" s="46" t="s">
         <v>153</v>
       </c>
-      <c r="I1013" s="37">
-        <v>36000</v>
-      </c>
+      <c r="I1013" s="37"/>
       <c r="J1013" s="37"/>
       <c r="K1013" s="37"/>
       <c r="L1013" s="37"/>
@@ -35632,9 +35148,7 @@
       <c r="H1015" s="46" t="s">
         <v>154</v>
       </c>
-      <c r="I1015" s="37">
-        <v>312000</v>
-      </c>
+      <c r="I1015" s="37"/>
       <c r="J1015" s="37"/>
       <c r="K1015" s="37"/>
       <c r="L1015" s="37"/>
@@ -35754,7 +35268,7 @@
       </c>
       <c r="I1019" s="5">
         <f>SUM(I966:I1015)</f>
-        <v>5579200</v>
+        <v>2633600</v>
       </c>
       <c r="J1019" s="5"/>
       <c r="K1019" s="5"/>
@@ -35799,9 +35313,7 @@
       <c r="H1021" s="46" t="s">
         <v>157</v>
       </c>
-      <c r="I1021" s="37">
-        <v>750000</v>
-      </c>
+      <c r="I1021" s="37"/>
       <c r="J1021" s="37"/>
       <c r="K1021" s="37"/>
       <c r="L1021" s="37"/>
@@ -35857,9 +35369,7 @@
       <c r="H1023" s="46" t="s">
         <v>158</v>
       </c>
-      <c r="I1023" s="37">
-        <v>200000</v>
-      </c>
+      <c r="I1023" s="37"/>
       <c r="J1023" s="37"/>
       <c r="K1023" s="37"/>
       <c r="L1023" s="37"/>
@@ -35915,9 +35425,7 @@
       <c r="H1025" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="I1025" s="37">
-        <v>200000</v>
-      </c>
+      <c r="I1025" s="37"/>
       <c r="J1025" s="37"/>
       <c r="K1025" s="37"/>
       <c r="L1025" s="37"/>
@@ -35967,9 +35475,7 @@
       <c r="H1027" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="I1027" s="37">
-        <v>100000</v>
-      </c>
+      <c r="I1027" s="37"/>
       <c r="J1027" s="37"/>
       <c r="K1027" s="37"/>
       <c r="L1027" s="37"/>
@@ -36019,9 +35525,7 @@
       <c r="H1029" s="46" t="s">
         <v>161</v>
       </c>
-      <c r="I1029" s="37">
-        <v>80000</v>
-      </c>
+      <c r="I1029" s="37"/>
       <c r="J1029" s="37"/>
       <c r="K1029" s="37"/>
       <c r="L1029" s="37"/>
@@ -36100,9 +35604,7 @@
       <c r="H1032" s="46" t="s">
         <v>162</v>
       </c>
-      <c r="I1032" s="37">
-        <v>200000</v>
-      </c>
+      <c r="I1032" s="37"/>
       <c r="J1032" s="37"/>
       <c r="K1032" s="37"/>
       <c r="L1032" s="37"/>
@@ -36152,9 +35654,7 @@
       <c r="H1034" s="46" t="s">
         <v>163</v>
       </c>
-      <c r="I1034" s="37">
-        <v>150000</v>
-      </c>
+      <c r="I1034" s="37"/>
       <c r="J1034" s="37"/>
       <c r="K1034" s="37"/>
       <c r="L1034" s="37"/>
@@ -36204,9 +35704,7 @@
       <c r="H1036" s="46" t="s">
         <v>164</v>
       </c>
-      <c r="I1036" s="37">
-        <v>300000</v>
-      </c>
+      <c r="I1036" s="37"/>
       <c r="J1036" s="37"/>
       <c r="K1036" s="37"/>
       <c r="L1036" s="37"/>
@@ -36256,9 +35754,7 @@
       <c r="H1038" s="46" t="s">
         <v>165</v>
       </c>
-      <c r="I1038" s="37">
-        <v>350000</v>
-      </c>
+      <c r="I1038" s="37"/>
       <c r="J1038" s="37"/>
       <c r="K1038" s="37"/>
       <c r="L1038" s="37"/>
@@ -36308,9 +35804,7 @@
       <c r="H1040" s="46" t="s">
         <v>166</v>
       </c>
-      <c r="I1040" s="37">
-        <v>950000</v>
-      </c>
+      <c r="I1040" s="37"/>
       <c r="J1040" s="37"/>
       <c r="K1040" s="37"/>
       <c r="L1040" s="37"/>
@@ -36362,9 +35856,7 @@
       <c r="H1042" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="I1042" s="37">
-        <v>1500000</v>
-      </c>
+      <c r="I1042" s="37"/>
       <c r="J1042" s="37"/>
       <c r="K1042" s="37"/>
       <c r="L1042" s="37"/>
@@ -36414,9 +35906,7 @@
       <c r="H1044" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="I1044" s="37">
-        <v>200000</v>
-      </c>
+      <c r="I1044" s="37"/>
       <c r="J1044" s="37"/>
       <c r="K1044" s="37"/>
       <c r="L1044" s="37"/>
@@ -36813,7 +36303,7 @@
       </c>
       <c r="I1061" s="3">
         <f>I1019+I1046+I1060</f>
-        <v>10559200</v>
+        <v>7613600</v>
       </c>
       <c r="J1061" s="3"/>
       <c r="K1061" s="3"/>
@@ -36881,9 +36371,7 @@
       <c r="H1064" s="46" t="s">
         <v>141</v>
       </c>
-      <c r="I1064" s="37">
-        <v>400000</v>
-      </c>
+      <c r="I1064" s="37"/>
       <c r="J1064" s="37"/>
       <c r="K1064" s="37"/>
       <c r="L1064" s="37"/>
@@ -37091,9 +36579,7 @@
       <c r="H1070" s="46" t="s">
         <v>142</v>
       </c>
-      <c r="I1070" s="37">
-        <v>82200</v>
-      </c>
+      <c r="I1070" s="37"/>
       <c r="J1070" s="37"/>
       <c r="K1070" s="37"/>
       <c r="L1070" s="37"/>
@@ -37301,9 +36787,7 @@
       <c r="H1076" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="I1076" s="37">
-        <v>4800</v>
-      </c>
+      <c r="I1076" s="37"/>
       <c r="J1076" s="37"/>
       <c r="K1076" s="37"/>
       <c r="L1076" s="37"/>
@@ -37390,9 +36874,7 @@
       <c r="H1079" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="I1079" s="37">
-        <v>12000</v>
-      </c>
+      <c r="I1079" s="37"/>
       <c r="J1079" s="37"/>
       <c r="K1079" s="37"/>
       <c r="L1079" s="37"/>
@@ -37489,9 +36971,7 @@
       <c r="H1082" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="I1082" s="37">
-        <v>0</v>
-      </c>
+      <c r="I1082" s="37"/>
       <c r="J1082" s="37"/>
       <c r="K1082" s="37"/>
       <c r="L1082" s="37"/>
@@ -37578,9 +37058,7 @@
       <c r="H1085" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="I1085" s="37">
-        <v>90800</v>
-      </c>
+      <c r="I1085" s="37"/>
       <c r="J1085" s="37"/>
       <c r="K1085" s="37"/>
       <c r="L1085" s="37"/>
@@ -37749,9 +37227,7 @@
       <c r="H1090" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="I1090" s="37">
-        <v>90000</v>
-      </c>
+      <c r="I1090" s="37"/>
       <c r="J1090" s="37"/>
       <c r="K1090" s="37"/>
       <c r="L1090" s="37"/>
@@ -37920,9 +37396,7 @@
       <c r="H1095" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="I1095" s="37">
-        <v>53400</v>
-      </c>
+      <c r="I1095" s="37"/>
       <c r="J1095" s="37"/>
       <c r="K1095" s="37"/>
       <c r="L1095" s="37"/>
@@ -38077,9 +37551,7 @@
       <c r="H1100" s="46" t="s">
         <v>148</v>
       </c>
-      <c r="I1100" s="37">
-        <v>2000</v>
-      </c>
+      <c r="I1100" s="37"/>
       <c r="J1100" s="37"/>
       <c r="K1100" s="37"/>
       <c r="L1100" s="37"/>
@@ -38205,9 +37677,7 @@
       <c r="H1104" s="46" t="s">
         <v>149</v>
       </c>
-      <c r="I1104" s="37">
-        <v>20000</v>
-      </c>
+      <c r="I1104" s="37"/>
       <c r="J1104" s="37"/>
       <c r="K1104" s="37"/>
       <c r="L1104" s="37"/>
@@ -38304,9 +37774,7 @@
       <c r="H1107" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="I1107" s="37">
-        <v>0</v>
-      </c>
+      <c r="I1107" s="37"/>
       <c r="J1107" s="37"/>
       <c r="K1107" s="37"/>
       <c r="L1107" s="37"/>
@@ -38393,9 +37861,7 @@
       <c r="H1110" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="I1110" s="37">
-        <v>0</v>
-      </c>
+      <c r="I1110" s="37"/>
       <c r="J1110" s="37"/>
       <c r="K1110" s="37"/>
       <c r="L1110" s="37"/>
@@ -38482,9 +37948,7 @@
       <c r="H1113" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="I1113" s="37">
-        <v>0</v>
-      </c>
+      <c r="I1113" s="37"/>
       <c r="J1113" s="37"/>
       <c r="K1113" s="37"/>
       <c r="L1113" s="37"/>
@@ -38571,9 +38035,7 @@
       <c r="H1116" s="46" t="s">
         <v>153</v>
       </c>
-      <c r="I1116" s="37">
-        <v>0</v>
-      </c>
+      <c r="I1116" s="37"/>
       <c r="J1116" s="37"/>
       <c r="K1116" s="37"/>
       <c r="L1116" s="37"/>
@@ -38660,9 +38122,7 @@
       <c r="H1119" s="46" t="s">
         <v>154</v>
       </c>
-      <c r="I1119" s="37">
-        <v>55000</v>
-      </c>
+      <c r="I1119" s="37"/>
       <c r="J1119" s="37"/>
       <c r="K1119" s="37"/>
       <c r="L1119" s="37"/>
@@ -38833,7 +38293,7 @@
       </c>
       <c r="I1124" s="5">
         <f>SUM(I1064:I1119)</f>
-        <v>1565400</v>
+        <v>755200</v>
       </c>
       <c r="J1124" s="5"/>
       <c r="K1124" s="5"/>
@@ -38878,9 +38338,7 @@
       <c r="H1126" s="46" t="s">
         <v>157</v>
       </c>
-      <c r="I1126" s="37">
-        <v>5000</v>
-      </c>
+      <c r="I1126" s="37"/>
       <c r="J1126" s="37"/>
       <c r="K1126" s="37"/>
       <c r="L1126" s="37"/>
@@ -38940,9 +38398,7 @@
       <c r="H1128" s="46" t="s">
         <v>158</v>
       </c>
-      <c r="I1128" s="37">
-        <v>0</v>
-      </c>
+      <c r="I1128" s="37"/>
       <c r="J1128" s="37"/>
       <c r="K1128" s="37"/>
       <c r="L1128" s="37"/>
@@ -38963,9 +38419,7 @@
       <c r="H1129" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="I1129" s="37">
-        <v>0</v>
-      </c>
+      <c r="I1129" s="37"/>
       <c r="J1129" s="37"/>
       <c r="K1129" s="37"/>
       <c r="L1129" s="37"/>
@@ -38986,9 +38440,7 @@
       <c r="H1130" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="I1130" s="37">
-        <v>0</v>
-      </c>
+      <c r="I1130" s="37"/>
       <c r="J1130" s="37"/>
       <c r="K1130" s="37"/>
       <c r="L1130" s="37"/>
@@ -39009,9 +38461,7 @@
       <c r="H1131" s="46" t="s">
         <v>161</v>
       </c>
-      <c r="I1131" s="37">
-        <v>10000</v>
-      </c>
+      <c r="I1131" s="37"/>
       <c r="J1131" s="37"/>
       <c r="K1131" s="37"/>
       <c r="L1131" s="37"/>
@@ -39069,9 +38519,7 @@
       <c r="H1133" s="46" t="s">
         <v>162</v>
       </c>
-      <c r="I1133" s="37">
-        <v>0</v>
-      </c>
+      <c r="I1133" s="37"/>
       <c r="J1133" s="37"/>
       <c r="K1133" s="37"/>
       <c r="L1133" s="37"/>
@@ -39092,9 +38540,7 @@
       <c r="H1134" s="46" t="s">
         <v>163</v>
       </c>
-      <c r="I1134" s="37">
-        <v>400000</v>
-      </c>
+      <c r="I1134" s="37"/>
       <c r="J1134" s="37"/>
       <c r="K1134" s="37"/>
       <c r="L1134" s="37"/>
@@ -39152,9 +38598,7 @@
       <c r="H1136" s="46" t="s">
         <v>164</v>
       </c>
-      <c r="I1136" s="37">
-        <v>0</v>
-      </c>
+      <c r="I1136" s="37"/>
       <c r="J1136" s="37"/>
       <c r="K1136" s="37"/>
       <c r="L1136" s="37"/>
@@ -39175,9 +38619,7 @@
       <c r="H1137" s="46" t="s">
         <v>165</v>
       </c>
-      <c r="I1137" s="37">
-        <v>0</v>
-      </c>
+      <c r="I1137" s="37"/>
       <c r="J1137" s="37"/>
       <c r="K1137" s="37"/>
       <c r="L1137" s="37"/>
@@ -39198,9 +38640,7 @@
       <c r="H1138" s="46" t="s">
         <v>166</v>
       </c>
-      <c r="I1138" s="37">
-        <v>0</v>
-      </c>
+      <c r="I1138" s="37"/>
       <c r="J1138" s="37"/>
       <c r="K1138" s="37"/>
       <c r="L1138" s="37"/>
@@ -39221,9 +38661,7 @@
       <c r="H1139" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="I1139" s="37">
-        <v>0</v>
-      </c>
+      <c r="I1139" s="37"/>
       <c r="J1139" s="37"/>
       <c r="K1139" s="37"/>
       <c r="L1139" s="37"/>
@@ -39244,9 +38682,7 @@
       <c r="H1140" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="I1140" s="37">
-        <v>0</v>
-      </c>
+      <c r="I1140" s="37"/>
       <c r="J1140" s="37"/>
       <c r="K1140" s="37"/>
       <c r="L1140" s="37"/>
@@ -39269,7 +38705,7 @@
       </c>
       <c r="I1141" s="5">
         <f>SUM(I1126:I1140)</f>
-        <v>701000</v>
+        <v>286000</v>
       </c>
       <c r="J1141" s="5"/>
       <c r="K1141" s="5"/>
@@ -39616,7 +39052,7 @@
       </c>
       <c r="I1156" s="3">
         <f>I1124+I1141+I1155</f>
-        <v>2266400</v>
+        <v>1041200</v>
       </c>
       <c r="J1156" s="3"/>
       <c r="K1156" s="3"/>
@@ -39684,9 +39120,7 @@
       <c r="H1159" s="46" t="s">
         <v>179</v>
       </c>
-      <c r="I1159" s="52">
-        <v>300000</v>
-      </c>
+      <c r="I1159" s="52"/>
       <c r="J1159" s="52"/>
       <c r="K1159" s="52"/>
       <c r="L1159" s="52"/>
@@ -39966,9 +39400,7 @@
       <c r="H1167" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="I1167" s="52">
-        <v>649000</v>
-      </c>
+      <c r="I1167" s="52"/>
       <c r="J1167" s="52"/>
       <c r="K1167" s="52"/>
       <c r="L1167" s="52"/>
@@ -40254,9 +39686,7 @@
       <c r="H1175" s="46" t="s">
         <v>181</v>
       </c>
-      <c r="I1175" s="52">
-        <v>131000</v>
-      </c>
+      <c r="I1175" s="52"/>
       <c r="J1175" s="52"/>
       <c r="K1175" s="52"/>
       <c r="L1175" s="52"/>
@@ -40473,9 +39903,7 @@
       <c r="H1182" s="46" t="s">
         <v>182</v>
       </c>
-      <c r="I1182" s="52">
-        <v>26000</v>
-      </c>
+      <c r="I1182" s="52"/>
       <c r="J1182" s="52"/>
       <c r="K1182" s="52"/>
       <c r="L1182" s="52"/>
@@ -40556,9 +39984,7 @@
       <c r="H1185" s="46" t="s">
         <v>183</v>
       </c>
-      <c r="I1185" s="52">
-        <v>295000</v>
-      </c>
+      <c r="I1185" s="52"/>
       <c r="J1185" s="52"/>
       <c r="K1185" s="52"/>
       <c r="L1185" s="52"/>
@@ -40836,9 +40262,7 @@
       <c r="H1193" s="46" t="s">
         <v>184</v>
       </c>
-      <c r="I1193" s="37">
-        <v>102500</v>
-      </c>
+      <c r="I1193" s="37"/>
       <c r="J1193" s="37"/>
       <c r="K1193" s="37"/>
       <c r="L1193" s="37"/>
@@ -41102,9 +40526,7 @@
       <c r="H1201" s="46" t="s">
         <v>185</v>
       </c>
-      <c r="I1201" s="37">
-        <v>50000</v>
-      </c>
+      <c r="I1201" s="37"/>
       <c r="J1201" s="37"/>
       <c r="K1201" s="37"/>
       <c r="L1201" s="37"/>
@@ -41372,9 +40794,7 @@
       <c r="H1209" s="46" t="s">
         <v>186</v>
       </c>
-      <c r="I1209" s="37">
-        <v>240500</v>
-      </c>
+      <c r="I1209" s="37"/>
       <c r="J1209" s="37"/>
       <c r="K1209" s="37"/>
       <c r="L1209" s="37"/>
@@ -41652,9 +41072,7 @@
       <c r="H1217" s="46" t="s">
         <v>187</v>
       </c>
-      <c r="I1217" s="37">
-        <v>4000</v>
-      </c>
+      <c r="I1217" s="37"/>
       <c r="J1217" s="37"/>
       <c r="K1217" s="37"/>
       <c r="L1217" s="37"/>
@@ -41836,9 +41254,7 @@
       <c r="H1223" s="46" t="s">
         <v>188</v>
       </c>
-      <c r="I1223" s="37">
-        <v>19000</v>
-      </c>
+      <c r="I1223" s="37"/>
       <c r="J1223" s="37"/>
       <c r="K1223" s="37"/>
       <c r="L1223" s="37"/>
@@ -41952,9 +41368,7 @@
       <c r="H1227" s="46" t="s">
         <v>189</v>
       </c>
-      <c r="I1227" s="37">
-        <v>37000</v>
-      </c>
+      <c r="I1227" s="37"/>
       <c r="J1227" s="37"/>
       <c r="K1227" s="37"/>
       <c r="L1227" s="37"/>
@@ -42181,7 +41595,7 @@
       </c>
       <c r="I1234" s="5">
         <f>SUM(I1159:I1227)</f>
-        <v>3671000</v>
+        <v>1817000</v>
       </c>
       <c r="J1234" s="5"/>
       <c r="K1234" s="5"/>
@@ -42205,7 +41619,7 @@
       </c>
       <c r="I1235" s="3">
         <f>I1234</f>
-        <v>3671000</v>
+        <v>1817000</v>
       </c>
       <c r="J1235" s="3"/>
       <c r="K1235" s="3"/>
@@ -42273,9 +41687,7 @@
       <c r="H1238" s="46" t="s">
         <v>179</v>
       </c>
-      <c r="I1238" s="52">
-        <v>167000</v>
-      </c>
+      <c r="I1238" s="52"/>
       <c r="J1238" s="52"/>
       <c r="K1238" s="52"/>
       <c r="L1238" s="52"/>
@@ -42483,9 +41895,7 @@
       <c r="H1244" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="I1244" s="52">
-        <v>325000</v>
-      </c>
+      <c r="I1244" s="52"/>
       <c r="J1244" s="52"/>
       <c r="K1244" s="52"/>
       <c r="L1244" s="52"/>
@@ -42697,9 +42107,7 @@
       <c r="H1250" s="46" t="s">
         <v>181</v>
       </c>
-      <c r="I1250" s="52">
-        <v>117000</v>
-      </c>
+      <c r="I1250" s="52"/>
       <c r="J1250" s="52"/>
       <c r="K1250" s="52"/>
       <c r="L1250" s="52"/>
@@ -42899,9 +42307,7 @@
       <c r="H1256" s="46" t="s">
         <v>182</v>
       </c>
-      <c r="I1256" s="52">
-        <v>65000</v>
-      </c>
+      <c r="I1256" s="52"/>
       <c r="J1256" s="52"/>
       <c r="K1256" s="52"/>
       <c r="L1256" s="52"/>
@@ -43095,9 +42501,7 @@
       <c r="H1262" s="46" t="s">
         <v>183</v>
       </c>
-      <c r="I1262" s="52">
-        <v>107100</v>
-      </c>
+      <c r="I1262" s="52"/>
       <c r="J1262" s="52"/>
       <c r="K1262" s="52"/>
       <c r="L1262" s="52"/>
@@ -43303,9 +42707,7 @@
       <c r="H1268" s="46" t="s">
         <v>184</v>
       </c>
-      <c r="I1268" s="37">
-        <v>63000</v>
-      </c>
+      <c r="I1268" s="37"/>
       <c r="J1268" s="37"/>
       <c r="K1268" s="37"/>
       <c r="L1268" s="37"/>
@@ -43513,9 +42915,7 @@
       <c r="H1274" s="46" t="s">
         <v>185</v>
       </c>
-      <c r="I1274" s="37">
-        <v>54000</v>
-      </c>
+      <c r="I1274" s="37"/>
       <c r="J1274" s="37"/>
       <c r="K1274" s="37"/>
       <c r="L1274" s="37"/>
@@ -43719,9 +43119,7 @@
       <c r="H1280" s="46" t="s">
         <v>186</v>
       </c>
-      <c r="I1280" s="37">
-        <v>2982200</v>
-      </c>
+      <c r="I1280" s="37"/>
       <c r="J1280" s="37"/>
       <c r="K1280" s="37"/>
       <c r="L1280" s="37"/>
@@ -43927,9 +43325,7 @@
       <c r="H1286" s="46" t="s">
         <v>187</v>
       </c>
-      <c r="I1286" s="37">
-        <v>2000</v>
-      </c>
+      <c r="I1286" s="37"/>
       <c r="J1286" s="37"/>
       <c r="K1286" s="37"/>
       <c r="L1286" s="37"/>
@@ -44090,9 +43486,7 @@
       <c r="H1291" s="46" t="s">
         <v>188</v>
       </c>
-      <c r="I1291" s="37">
-        <v>4000</v>
-      </c>
+      <c r="I1291" s="37"/>
       <c r="J1291" s="37"/>
       <c r="K1291" s="37"/>
       <c r="L1291" s="37"/>
@@ -44218,9 +43612,7 @@
       <c r="H1295" s="46" t="s">
         <v>189</v>
       </c>
-      <c r="I1295" s="37">
-        <v>31000</v>
-      </c>
+      <c r="I1295" s="37"/>
       <c r="J1295" s="37"/>
       <c r="K1295" s="37"/>
       <c r="L1295" s="37"/>
@@ -44428,7 +43820,7 @@
       </c>
       <c r="I1301" s="5">
         <f>SUM(I1238:I1295)</f>
-        <v>7803600</v>
+        <v>3886300</v>
       </c>
       <c r="J1301" s="5"/>
       <c r="K1301" s="5"/>
@@ -44452,7 +43844,7 @@
       </c>
       <c r="I1302" s="3">
         <f>I1301</f>
-        <v>7803600</v>
+        <v>3886300</v>
       </c>
       <c r="J1302" s="3"/>
       <c r="K1302" s="3"/>
@@ -44522,9 +43914,7 @@
       <c r="H1305" s="46" t="s">
         <v>195</v>
       </c>
-      <c r="I1305" s="37">
-        <v>0</v>
-      </c>
+      <c r="I1305" s="37"/>
       <c r="J1305" s="37"/>
       <c r="K1305" s="37"/>
       <c r="L1305" s="37"/>
@@ -44547,9 +43937,7 @@
       <c r="H1306" s="46" t="s">
         <v>196</v>
       </c>
-      <c r="I1306" s="37">
-        <v>465900</v>
-      </c>
+      <c r="I1306" s="37"/>
       <c r="J1306" s="37"/>
       <c r="K1306" s="37"/>
       <c r="L1306" s="37"/>
@@ -44827,9 +44215,7 @@
       <c r="H1314" s="46" t="s">
         <v>197</v>
       </c>
-      <c r="I1314" s="37">
-        <v>793300</v>
-      </c>
+      <c r="I1314" s="37"/>
       <c r="J1314" s="37"/>
       <c r="K1314" s="37"/>
       <c r="L1314" s="37"/>
@@ -45113,9 +44499,7 @@
       <c r="H1322" s="29" t="s">
         <v>198</v>
       </c>
-      <c r="I1322" s="37">
-        <v>0</v>
-      </c>
+      <c r="I1322" s="37"/>
       <c r="J1322" s="37"/>
       <c r="K1322" s="37"/>
       <c r="L1322" s="37"/>
@@ -45231,9 +44615,7 @@
       <c r="H1327" s="46" t="s">
         <v>195</v>
       </c>
-      <c r="I1327" s="37">
-        <v>0</v>
-      </c>
+      <c r="I1327" s="37"/>
       <c r="J1327" s="37"/>
       <c r="K1327" s="37"/>
       <c r="L1327" s="37"/>
@@ -45256,9 +44638,7 @@
       <c r="H1328" s="46" t="s">
         <v>196</v>
       </c>
-      <c r="I1328" s="37">
-        <v>181000</v>
-      </c>
+      <c r="I1328" s="37"/>
       <c r="J1328" s="37"/>
       <c r="K1328" s="37"/>
       <c r="L1328" s="37"/>
@@ -45456,9 +44836,7 @@
       <c r="H1334" s="46" t="s">
         <v>197</v>
       </c>
-      <c r="I1334" s="37">
-        <v>517300</v>
-      </c>
+      <c r="I1334" s="37"/>
       <c r="J1334" s="37"/>
       <c r="K1334" s="37"/>
       <c r="L1334" s="37"/>
@@ -45672,9 +45050,7 @@
       <c r="H1340" s="29" t="s">
         <v>198</v>
       </c>
-      <c r="I1340" s="37">
-        <v>4329500</v>
-      </c>
+      <c r="I1340" s="37"/>
       <c r="J1340" s="37"/>
       <c r="K1340" s="37"/>
       <c r="L1340" s="37"/>

</xml_diff>